<commit_message>
Projectbrief done working on the integrated API.
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Week 6</t>
   </si>
@@ -474,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,4 +641,186 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="11" width="8.42578125" customWidth="1"/>
+    <col min="12" max="13" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="18" width="8.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MatchHandler works Core set prodApi to true, to activate request limiting
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Week 6</t>
   </si>
@@ -96,13 +96,31 @@
   </si>
   <si>
     <t>Week 23+</t>
+  </si>
+  <si>
+    <t>Opslaan van match data</t>
+  </si>
+  <si>
+    <t>Weergeven van match data</t>
+  </si>
+  <si>
+    <t>Verwerken van opgeslagen match data</t>
+  </si>
+  <si>
+    <t>Vormgeving van de inhoud</t>
+  </si>
+  <si>
+    <t>Grafische elementen van de applicatie afwerken</t>
+  </si>
+  <si>
+    <t>Fouten opsporen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +131,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,16 +188,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -187,9 +215,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +255,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +327,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -479,12 +507,12 @@
       <selection sqref="A1:S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -563,7 +591,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -586,14 +614,14 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -601,7 +629,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -609,21 +637,21 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -631,7 +659,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -645,29 +673,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
-    <col min="10" max="11" width="8.42578125" customWidth="1"/>
-    <col min="12" max="13" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" customWidth="1"/>
-    <col min="16" max="18" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" customWidth="1"/>
+    <col min="10" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="13" width="8.5546875" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" customWidth="1"/>
+    <col min="16" max="18" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -723,31 +751,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="5"/>
@@ -769,58 +797,99 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="S10" s="4"/>
+      <c r="S16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>